<commit_message>
update template expert fee
</commit_message>
<xml_diff>
--- a/public/templates/finance_template_expert_fee.xlsx
+++ b/public/templates/finance_template_expert_fee.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>序号</t>
   </si>
@@ -54,6 +54,9 @@
   </si>
   <si>
     <t>税费</t>
+  </si>
+  <si>
+    <t>备注</t>
   </si>
 </sst>
 </file>
@@ -61,10 +64,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -95,13 +98,43 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -115,6 +148,52 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
@@ -122,15 +201,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -144,82 +224,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -229,17 +233,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -258,31 +261,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -294,13 +393,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,133 +441,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -463,6 +466,15 @@
       </top>
       <bottom style="hair">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -500,23 +512,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -550,154 +547,160 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="32" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -1109,7 +1112,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1125,11 +1128,11 @@
     <col min="5" max="5" width="20.5666666666667" style="3"/>
     <col min="6" max="8" width="30.85" style="3"/>
     <col min="9" max="9" width="12.6583333333333" style="3"/>
-    <col min="10" max="13" width="16.2583333333333" style="2"/>
-    <col min="14" max="1027" width="9.08333333333333" style="4"/>
+    <col min="10" max="14" width="16.2583333333333" style="2"/>
+    <col min="15" max="1027" width="9.08333333333333" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="18" customHeight="1" spans="1:13">
+    <row r="1" s="1" customFormat="1" ht="18" customHeight="1" spans="1:14">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1168,6 +1171,9 @@
       </c>
       <c r="M1" s="5" t="s">
         <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>